<commit_message>
Geändert 234.xls neue Seite mit Frauenhofer Linien
</commit_message>
<xml_diff>
--- a/Praktikum/234 - Lichtquellen/Auswetung.xlsx
+++ b/Praktikum/234 - Lichtquellen/Auswetung.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Peakpos. [nm]</t>
   </si>
@@ -130,11 +131,65 @@
   <si>
     <t>0,8792±0,0009</t>
   </si>
+  <si>
+    <t>Linie</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>λ_lit [nm]</t>
+  </si>
+  <si>
+    <t>Δλ_exp [nm]</t>
+  </si>
+  <si>
+    <t>n.z.</t>
+  </si>
+  <si>
+    <t>Δλ [nm]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -319,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -339,6 +394,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -621,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
@@ -713,7 +775,7 @@
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="4">
-        <f t="shared" ref="M4:M8" si="1">(I4-K4)/(L4+J4)^2</f>
+        <f t="shared" ref="M4" si="1">(I4-K4)/(L4+J4)^2</f>
         <v>4.4444444444445077</v>
       </c>
       <c r="O4" s="2" t="s">
@@ -930,7 +992,7 @@
         <v>0.38</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" ref="M12:M16" si="2">(I13-K13)/(L13+J13)^2</f>
+        <f t="shared" ref="M13:M15" si="2">(I13-K13)/(L13+J13)^2</f>
         <v>6.9204152249135946</v>
       </c>
     </row>
@@ -1182,7 +1244,7 @@
         <v>0.42</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" ref="M25:M33" si="3">(I25-K25)/(L25+J25)^2</f>
+        <f t="shared" ref="M25:M30" si="3">(I25-K25)/(L25+J25)^2</f>
         <v>1.903628792385444</v>
       </c>
     </row>
@@ -1402,6 +1464,251 @@
       </c>
       <c r="F34" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="19">
+        <v>760.4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="19">
+        <v>759.4</v>
+      </c>
+      <c r="F3" s="20">
+        <f>((C3-E3)^2)^(1/2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="19">
+        <v>687.4</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="19">
+        <v>686.7</v>
+      </c>
+      <c r="F4" s="20">
+        <f t="shared" ref="F4:F14" si="0">((C4-E4)^2)^(1/2)</f>
+        <v>0.69999999999993179</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="19">
+        <v>656.2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="19">
+        <v>656.3</v>
+      </c>
+      <c r="F5" s="20">
+        <f t="shared" si="0"/>
+        <v>9.9999999999909051E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="19">
+        <v>589.5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="19">
+        <v>589.6</v>
+      </c>
+      <c r="F6" s="20">
+        <f t="shared" si="0"/>
+        <v>0.10000000000002274</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="19">
+        <v>589</v>
+      </c>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19">
+        <v>587.6</v>
+      </c>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="19">
+        <v>527</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="19">
+        <v>527</v>
+      </c>
+      <c r="F9" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="19">
+        <v>518.4</v>
+      </c>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="19">
+        <v>486.2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19">
+        <v>486.1</v>
+      </c>
+      <c r="F11" s="20">
+        <f t="shared" si="0"/>
+        <v>9.9999999999965894E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="19">
+        <v>430.8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19">
+        <v>430.8</v>
+      </c>
+      <c r="F12" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="19">
+        <v>396.9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="19">
+        <v>396.8</v>
+      </c>
+      <c r="F13" s="20">
+        <f t="shared" si="0"/>
+        <v>9.9999999999965894E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="22">
+        <v>393.6</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="22">
+        <v>393.4</v>
+      </c>
+      <c r="F14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20000000000004547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>